<commit_message>
All template is ready
</commit_message>
<xml_diff>
--- a/docs/Skill Up.xlsx
+++ b/docs/Skill Up.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Websites\upmyskill\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCF5EA27-CF72-4C89-AD9A-413E96336FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB197C25-F14D-4503-B65C-1FD96AEB97CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E733CE5-9A3E-443B-81BF-267A6435F5A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E733CE5-9A3E-443B-81BF-267A6435F5A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>About Us</t>
   </si>
@@ -83,12 +83,6 @@
   </si>
   <si>
     <t>Member Price</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time</t>
   </si>
   <si>
     <t>Duration</t>
@@ -252,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -284,12 +278,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -677,7 +665,7 @@
   <dimension ref="B2:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F8"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +677,7 @@
     <col min="9" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
@@ -708,7 +696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
@@ -716,37 +704,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="6" t="s">
         <v>13</v>
       </c>
@@ -761,226 +749,209 @@
       </c>
       <c r="G16" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="17" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="8"/>
       <c r="D17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1500</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="10">
-        <v>1500</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="9"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="9" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="18" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="8"/>
       <c r="D18" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E18" s="10">
         <v>1500</v>
       </c>
       <c r="F18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="9"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="9" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="19" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="11"/>
       <c r="D19" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E19" s="10">
         <v>1500</v>
       </c>
       <c r="F19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="12"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="12" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="20" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" s="10">
         <v>1500</v>
       </c>
       <c r="F20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="9"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="9" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="21" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="8"/>
       <c r="D21" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E21" s="10">
         <v>1500</v>
       </c>
       <c r="F21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="13"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="9" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="22" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="8"/>
       <c r="D22" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E22" s="10">
         <v>1500</v>
       </c>
       <c r="F22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="13"/>
       <c r="H22" s="9"/>
-      <c r="I22" s="9" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="23" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="11"/>
       <c r="D23" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E23" s="10">
         <v>1500</v>
       </c>
       <c r="F23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="14"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="12" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="24" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="8"/>
       <c r="D24" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E24" s="10">
         <v>1500</v>
       </c>
       <c r="F24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="9"/>
       <c r="H24" s="9"/>
-      <c r="I24" s="9" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="25" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="8"/>
       <c r="D25" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E25" s="10">
         <v>1500</v>
       </c>
       <c r="F25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="9"/>
       <c r="H25" s="9"/>
-      <c r="I25" s="9" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="26" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E26" s="10">
         <v>1500</v>
       </c>
       <c r="F26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="9"/>
       <c r="H26" s="9"/>
-      <c r="I26" s="9" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="27" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="11"/>
       <c r="D27" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E27" s="10">
         <v>1500</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="12"/>
+        <v>19</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="12" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="28" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="8"/>
       <c r="D28" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E28" s="10">
         <v>1500</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>